<commit_message>
compared relative spectral counts of go-linked peptides
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-p2-susvsink.xlsx
+++ b/analyses/etnp2017-p2-susvsink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFDF951C-431D-E446-97DA-0AE0CFC8AF64}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E74B5E-1CD3-2747-8008-5B41D35AE393}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32000" windowHeight="14540" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
+    <workbookView xWindow="1240" yWindow="1960" windowWidth="28040" windowHeight="19940" activeTab="1" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -394,12 +394,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -420,8 +426,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -434,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -444,12 +454,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11924,16 +11937,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13026,9 +13039,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FAA684-DE3F-5A4C-BBF8-96E0D7E03E10}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13038,59 +13051,59 @@
     <col min="21" max="21" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="80">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" s="7" customFormat="1" ht="80">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="8" t="s">
         <v>87</v>
       </c>
     </row>
@@ -13148,7 +13161,7 @@
       <c r="S2" s="4">
         <v>9495</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="5">
         <v>2881</v>
       </c>
       <c r="U2" s="4">
@@ -13209,7 +13222,7 @@
       <c r="S3" s="4">
         <v>3377</v>
       </c>
-      <c r="T3" s="6">
+      <c r="T3" s="5">
         <v>1294</v>
       </c>
       <c r="U3" s="4">
@@ -13270,7 +13283,7 @@
       <c r="S4" s="4">
         <v>2653</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="5">
         <v>1082</v>
       </c>
       <c r="U4" s="4">
@@ -14117,8 +14130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD91425-9F4A-7E4E-B842-3368493BFFE4}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14128,11 +14141,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -14201,11 +14214,11 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A7" s="1" t="s">

</xml_diff>

<commit_message>
unipept trees into susvsink analyses dirs
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-p2-susvsink.xlsx
+++ b/analyses/etnp2017-p2-susvsink.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E06E405-4613-0445-8F65-6D0B47B7EFAD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057482CD-2E38-4542-9AFF-8AEF4EE2DD92}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="460" windowWidth="25600" windowHeight="14640" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
+    <workbookView xWindow="-120" yWindow="460" windowWidth="25600" windowHeight="14640" activeTab="3" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
     <sheet name="100-965 comparison" sheetId="17" r:id="rId2"/>
-    <sheet name="ptm" sheetId="2" r:id="rId3"/>
+    <sheet name="PTMs" sheetId="2" r:id="rId3"/>
+    <sheet name="cyano peps" sheetId="18" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
   <si>
     <t>Sample running #</t>
   </si>
@@ -355,6 +356,24 @@
   <si>
     <t>Suspended GD/D&gt;0.3</t>
   </si>
+  <si>
+    <t>Matched to phyla or lower classification</t>
+  </si>
+  <si>
+    <t>100 m sinking</t>
+  </si>
+  <si>
+    <t>100 m suspended</t>
+  </si>
+  <si>
+    <t>965 m suspended</t>
+  </si>
+  <si>
+    <t>965 m sinking</t>
+  </si>
+  <si>
+    <t>spectral counts</t>
+  </si>
 </sst>
 </file>
 
@@ -397,7 +416,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +426,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -479,6 +504,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17273,9 +17302,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FAA684-DE3F-5A4C-BBF8-96E0D7E03E10}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14:I19"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R1" sqref="R1:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18364,7 +18393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD91425-9F4A-7E4E-B842-3368493BFFE4}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC53" sqref="AC53"/>
     </sheetView>
   </sheetViews>
@@ -18804,7 +18833,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19049,4 +19078,133 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFFF813-639D-5044-80D4-CB11098F52B7}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="14" customFormat="1" ht="32">
+      <c r="A1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="4">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4">
+        <v>9495</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2881</v>
+      </c>
+      <c r="E2" s="4">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="4">
+        <v>100</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3377</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1294</v>
+      </c>
+      <c r="E3" s="4">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="4">
+        <v>130</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2653</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1082</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="4">
+        <v>265</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2826</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1067</v>
+      </c>
+      <c r="E5" s="4">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made excel version of ja2 and ja14 peptide files
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-p2-susvsink.xlsx
+++ b/analyses/etnp2017-p2-susvsink.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115A94E8-BAD1-5941-B97B-909DA6710565}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F9BC9D-0753-6E49-884C-10F5B6D30EEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="460" windowWidth="25600" windowHeight="14640" activeTab="3" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27840" windowHeight="19320" activeTab="1" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="109">
   <si>
     <t>Sample running #</t>
   </si>
@@ -374,6 +379,9 @@
   <si>
     <t>spectral counts</t>
   </si>
+  <si>
+    <t>database peptides</t>
+  </si>
 </sst>
 </file>
 
@@ -524,9 +532,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -559,6 +564,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1337,6 +1345,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-B03D-504A-8A5A-26BE0B4C8EF6}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1552,6 +1563,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-B03D-504A-8A5A-26BE0B4C8EF6}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1654,6 +1668,9 @@
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>16780</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4914</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24005</c:v>
@@ -2040,6 +2057,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-37F1-2C48-8F53-4BE2EFD5A8C0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -2229,6 +2251,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-37F1-2C48-8F53-4BE2EFD5A8C0}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2457,6 +2482,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-37F1-2C48-8F53-4BE2EFD5A8C0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -2535,6 +2565,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-37F1-2C48-8F53-4BE2EFD5A8C0}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -3482,6 +3515,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-265B-4A49-A5C9-CFA0CED0C1D1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -3533,6 +3571,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-265B-4A49-A5C9-CFA0CED0C1D1}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -3778,6 +3819,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-265B-4A49-A5C9-CFA0CED0C1D1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -3829,6 +3875,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-265B-4A49-A5C9-CFA0CED0C1D1}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -3931,6 +3980,9 @@
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>16780</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4914</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24005</c:v>
@@ -6607,6 +6659,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BAC4-664E-9D73-84D66DA77D22}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -6658,6 +6715,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-BAC4-664E-9D73-84D66DA77D22}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6903,6 +6963,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-BAC4-664E-9D73-84D66DA77D22}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -6954,6 +7019,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-BAC4-664E-9D73-84D66DA77D22}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -8216,6 +8284,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-538B-FE46-A552-B1A997446742}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -8431,6 +8502,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-538B-FE46-A552-B1A997446742}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -17366,59 +17440,59 @@
     <col min="21" max="21" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="7" customFormat="1" ht="80">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="85">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -18443,10 +18517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD91425-9F4A-7E4E-B842-3368493BFFE4}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC53" sqref="AC53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -18455,14 +18529,14 @@
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="50" customHeight="1">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -18481,22 +18555,25 @@
       <c r="G2" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" s="11" customFormat="1" ht="18" customHeight="1">
-      <c r="A3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="11">
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="18" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
         <v>50</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>1285</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -18518,8 +18595,11 @@
       <c r="G4">
         <v>21252</v>
       </c>
+      <c r="H4">
+        <v>2159</v>
+      </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -18533,7 +18613,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -18547,7 +18627,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -18561,7 +18641,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -18583,8 +18663,11 @@
       <c r="G8">
         <v>15893</v>
       </c>
+      <c r="H8">
+        <v>160</v>
+      </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -18598,14 +18681,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
     </row>
-    <row r="12" spans="1:7" ht="48">
+    <row r="12" spans="1:8" ht="51">
       <c r="A12" s="1" t="s">
         <v>91</v>
       </c>
@@ -18626,59 +18709,59 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13">
         <v>50</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10">
+      <c r="C13" s="10"/>
+      <c r="D13" s="9">
         <v>1.5</v>
       </c>
       <c r="E13">
         <v>438</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>22</v>
       </c>
       <c r="B14">
         <v>100</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>1.5</v>
       </c>
       <c r="E14">
         <v>327</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>23</v>
       </c>
       <c r="B15">
         <v>130</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>1.5</v>
       </c>
       <c r="E15">
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>24</v>
       </c>
       <c r="B16">
         <v>265</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>1.5</v>
       </c>
       <c r="E16">
@@ -18692,7 +18775,7 @@
       <c r="B17">
         <v>300</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>1.5</v>
       </c>
       <c r="E17">
@@ -18706,7 +18789,7 @@
       <c r="B18">
         <v>1200</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>1.5</v>
       </c>
       <c r="E18">
@@ -18714,11 +18797,11 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A22" s="1" t="s">
@@ -18767,6 +18850,9 @@
       <c r="E24">
         <v>184</v>
       </c>
+      <c r="G24">
+        <v>4914</v>
+      </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
@@ -18791,14 +18877,14 @@
         <v>24005</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="7" t="s">
+    <row r="30" spans="1:7" ht="17">
+      <c r="A30" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -18895,7 +18981,7 @@
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="32">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="34">
       <c r="A1" s="3" t="s">
         <v>64</v>
       </c>
@@ -19136,7 +19222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFFF813-639D-5044-80D4-CB11098F52B7}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -19150,94 +19236,94 @@
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" ht="33" thickBot="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:6" s="12" customFormat="1" ht="35" thickBot="1">
+      <c r="A1" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="17">
         <v>50</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="17">
         <v>9495</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="17">
         <v>2881</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="17">
         <v>18</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>100</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="18">
         <v>3377</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="18">
         <v>1294</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="18">
         <v>14</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>130</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="18">
         <v>2653</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="18">
         <v>1082</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="18">
         <v>0</v>
       </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>265</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>2826</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <v>1067</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <v>7</v>
       </c>
       <c r="F5" s="4"/>

</xml_diff>

<commit_message>
updated susvsink metagomics notebook
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-p2-susvsink.xlsx
+++ b/analyses/etnp2017-p2-susvsink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10DB5B7-962C-B74E-8BC7-49C803327701}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F706C5A5-01CF-AE4C-B0D3-97E3FEE7A58B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="940" windowWidth="34860" windowHeight="14740" activeTab="1" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
+    <workbookView xWindow="1580" yWindow="1300" windowWidth="27840" windowHeight="19320" activeTab="3" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="114">
   <si>
     <t>Sample running #</t>
   </si>
@@ -362,9 +362,6 @@
     <t>Suspended GD/D&gt;0.3</t>
   </si>
   <si>
-    <t>Matched to phyla or lower classification</t>
-  </si>
-  <si>
     <t>100 m sinking</t>
   </si>
   <si>
@@ -377,20 +374,35 @@
     <t>965 m sinking</t>
   </si>
   <si>
-    <t>spectral counts</t>
-  </si>
-  <si>
     <t>database peptides</t>
   </si>
   <si>
     <t># MS spectra</t>
+  </si>
+  <si>
+    <t>de novo peptides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matched to phyla or better </t>
+  </si>
+  <si>
+    <t>specific cyanobacterial peptides</t>
+  </si>
+  <si>
+    <t>Table 1: DNO peptides</t>
+  </si>
+  <si>
+    <t>% cyano peptides modified</t>
+  </si>
+  <si>
+    <t># spectra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -426,6 +438,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -447,7 +465,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -468,19 +486,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -524,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -554,22 +559,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -26944,7 +26946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD91425-9F4A-7E4E-B842-3368493BFFE4}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BL8" sqref="BL8"/>
     </sheetView>
   </sheetViews>
@@ -26955,11 +26957,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -26981,10 +26983,10 @@
         <v>99</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="10" customFormat="1" ht="18" customHeight="1">
@@ -27226,11 +27228,11 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="51">
       <c r="A16" s="1" t="s">
@@ -27253,10 +27255,10 @@
         <v>99</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -27382,11 +27384,11 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A26" s="1" t="s">
@@ -27408,10 +27410,10 @@
         <v>99</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -27829,127 +27831,223 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFFF813-639D-5044-80D4-CB11098F52B7}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" ht="35" thickBot="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" s="12" customFormat="1" ht="88" customHeight="1" thickBot="1">
+      <c r="A1" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28">
+      <c r="A2" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="16">
+        <v>9495</v>
+      </c>
+      <c r="C2" s="16">
+        <v>2881</v>
+      </c>
+      <c r="D2" s="16">
+        <v>18</v>
+      </c>
+      <c r="E2" s="16">
+        <v>539</v>
+      </c>
+      <c r="F2" s="16">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28">
+      <c r="A3" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>107</v>
+      <c r="B3" s="18">
+        <v>3377</v>
+      </c>
+      <c r="C3" s="18">
+        <v>1294</v>
+      </c>
+      <c r="D3" s="18">
+        <v>14</v>
+      </c>
+      <c r="E3" s="18">
+        <v>245</v>
+      </c>
+      <c r="F3" s="18">
+        <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="15" t="s">
+    <row r="4" spans="1:6" ht="28">
+      <c r="A4" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="17">
-        <v>50</v>
-      </c>
-      <c r="C2" s="17">
-        <v>9495</v>
-      </c>
-      <c r="D2" s="17">
-        <v>2881</v>
-      </c>
-      <c r="E2" s="17">
-        <v>18</v>
-      </c>
-      <c r="F2" s="4"/>
+      <c r="B4" s="18">
+        <v>2653</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1082</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="18">
-        <v>100</v>
-      </c>
-      <c r="C3" s="18">
-        <v>3377</v>
-      </c>
-      <c r="D3" s="18">
-        <v>1294</v>
-      </c>
-      <c r="E3" s="18">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="14" t="s">
+    <row r="5" spans="1:6" ht="28">
+      <c r="A5" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="18">
-        <v>130</v>
-      </c>
-      <c r="C4" s="18">
-        <v>2653</v>
-      </c>
-      <c r="D4" s="18">
-        <v>1082</v>
-      </c>
-      <c r="E4" s="18">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="14" t="s">
-        <v>106</v>
-      </c>
       <c r="B5" s="18">
-        <v>265</v>
+        <v>2826</v>
       </c>
       <c r="C5" s="18">
-        <v>2826</v>
+        <v>1067</v>
       </c>
       <c r="D5" s="18">
-        <v>1067</v>
+        <v>7</v>
       </c>
       <c r="E5" s="18">
-        <v>7</v>
-      </c>
-      <c r="F5" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="F5" s="18">
+        <v>51.9</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="88" thickBot="1">
+      <c r="A9" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28">
+      <c r="A10" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="16">
+        <v>2159</v>
+      </c>
+      <c r="C10" s="16">
+        <v>784</v>
+      </c>
+      <c r="D10" s="16">
+        <v>482</v>
+      </c>
+      <c r="E10" s="16">
+        <v>4533</v>
+      </c>
+      <c r="F10" s="16">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28">
+      <c r="A11" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="18">
+        <v>591</v>
+      </c>
+      <c r="C11" s="18">
+        <v>235</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28">
+      <c r="A12" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="18">
+        <v>160</v>
+      </c>
+      <c r="C12" s="18">
+        <v>52</v>
+      </c>
+      <c r="D12" s="18">
+        <v>0</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:6" ht="28">
+      <c r="A13" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="18">
+        <v>1153</v>
+      </c>
+      <c r="C13" s="18">
+        <v>392</v>
+      </c>
+      <c r="D13" s="18">
+        <v>0</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0</v>
+      </c>
+      <c r="F13" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
replotted peaks dno vs db peptide mods
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-p2-susvsink.xlsx
+++ b/analyses/etnp2017-p2-susvsink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F706C5A5-01CF-AE4C-B0D3-97E3FEE7A58B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905E534B-2A0E-8C42-85CB-EFCB7A8FA1CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1300" windowWidth="27840" windowHeight="19320" activeTab="3" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
+    <workbookView xWindow="1600" yWindow="4240" windowWidth="27840" windowHeight="14640" activeTab="1" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="115">
   <si>
     <t>Sample running #</t>
   </si>
@@ -396,6 +396,9 @@
   </si>
   <si>
     <t># spectra</t>
+  </si>
+  <si>
+    <t>Specific cyanobacterial peptides de novo</t>
   </si>
 </sst>
 </file>
@@ -8766,6 +8769,1412 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" i="0"/>
+              <a:t>de novo cyanobacteria specific peptides</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28945882352941171"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>suspended (0.3-2.7 um)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B0F0">
+                <a:alpha val="57000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>18</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-04EB-A94A-BA72-9D5CAE5EBE38}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>0</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-04EB-A94A-BA72-9D5CAE5EBE38}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$D$4,'100-965 comparison'!$D$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$B$4,'100-965 comparison'!$B$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$J$4,'100-965 comparison'!$J$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-04EB-A94A-BA72-9D5CAE5EBE38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>sinking</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050">
+                <a:alpha val="57000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050">
+                  <a:alpha val="57000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-04EB-A94A-BA72-9D5CAE5EBE38}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>14</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-04EB-A94A-BA72-9D5CAE5EBE38}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>7</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-04EB-A94A-BA72-9D5CAE5EBE38}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$D$27,'100-965 comparison'!$D$29)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$B$27,'100-965 comparison'!$B$29)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$J$27,'100-965 comparison'!$J$29)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-04EB-A94A-BA72-9D5CAE5EBE38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="679452944"/>
+        <c:axId val="674288448"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="679452944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.5"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674288448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="674288448"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="1200"/>
+          <c:min val="-100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="679452944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="21000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="49000">
+              <a:schemeClr val="accent4">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="57000">
+              <a:schemeClr val="accent4">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+                <a:alpha val="46000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="70000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" i="0"/>
+              <a:t>database cyanobacteria specific peptides</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.29887058823529411"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>suspended (0.3-2.7 um)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B0F0">
+                <a:alpha val="57000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>18</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-00C0-6344-99DA-6A11A9519028}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>0</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-00C0-6344-99DA-6A11A9519028}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$D$4,'100-965 comparison'!$D$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$B$4,'100-965 comparison'!$B$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$J$4,'100-965 comparison'!$J$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-00C0-6344-99DA-6A11A9519028}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>sinking</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050">
+                <a:alpha val="57000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050">
+                  <a:alpha val="57000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-00C0-6344-99DA-6A11A9519028}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>14</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-00C0-6344-99DA-6A11A9519028}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>7</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-00C0-6344-99DA-6A11A9519028}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$D$27,'100-965 comparison'!$D$29)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$B$27,'100-965 comparison'!$B$29)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>('100-965 comparison'!$J$27,'100-965 comparison'!$J$29)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-00C0-6344-99DA-6A11A9519028}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="679452944"/>
+        <c:axId val="674288448"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="679452944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.5"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674288448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="674288448"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="1200"/>
+          <c:min val="-100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="679452944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="21000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+            <a:gs pos="49000">
+              <a:schemeClr val="accent4">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="57000">
+              <a:schemeClr val="accent4">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+                <a:alpha val="46000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="70000">
+              <a:schemeClr val="bg1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -13747,6 +15156,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17783,6 +19272,1076 @@
 </file>
 
 <file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -23242,12 +25801,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.26781</cdr:x>
-      <cdr:y>0.05988</cdr:y>
+      <cdr:x>0.21291</cdr:x>
+      <cdr:y>0.06119</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.43467</cdr:x>
-      <cdr:y>0.13255</cdr:y>
+      <cdr:x>0.48471</cdr:x>
+      <cdr:y>0.13386</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -23262,8 +25821,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2168263" y="580283"/>
-          <a:ext cx="1350940" cy="704180"/>
+          <a:off x="1723762" y="592983"/>
+          <a:ext cx="2200537" cy="704180"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -23282,7 +25841,457 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>suspended </a:t>
+            <a:t>small suspended </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.72744</cdr:x>
+      <cdr:y>0.06558</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.8943</cdr:x>
+      <cdr:y>0.13825</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DCA4D0-3347-C647-BC53-7E8414DB7BEE}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5889542" y="635517"/>
+          <a:ext cx="1350941" cy="704179"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>sinking </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04235</cdr:x>
+      <cdr:y>0.03408</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.18039</cdr:x>
+      <cdr:y>0.12189</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B7BD7A-571A-8142-9BE5-97BC8F34A850}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="342900" y="330200"/>
+          <a:ext cx="1117600" cy="850900"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.22703</cdr:x>
+      <cdr:y>0.06512</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.47373</cdr:x>
+      <cdr:y>0.13779</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AD5E656-48EB-5247-A3D6-D31E1B0020CA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1838056" y="631043"/>
+          <a:ext cx="1997343" cy="704180"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>small suspended </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.72744</cdr:x>
+      <cdr:y>0.06558</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.8943</cdr:x>
+      <cdr:y>0.13825</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DCA4D0-3347-C647-BC53-7E8414DB7BEE}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5889542" y="635517"/>
+          <a:ext cx="1350941" cy="704179"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>sinking </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04235</cdr:x>
+      <cdr:y>0.03408</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.18039</cdr:x>
+      <cdr:y>0.12189</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B7BD7A-571A-8142-9BE5-97BC8F34A850}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="342900" y="330200"/>
+          <a:ext cx="1117600" cy="850900"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.22703</cdr:x>
+      <cdr:y>0.06512</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.47373</cdr:x>
+      <cdr:y>0.13779</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AD5E656-48EB-5247-A3D6-D31E1B0020CA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1838056" y="631043"/>
+          <a:ext cx="1997343" cy="704180"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>small suspended </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -23838,6 +26847,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>82</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E2E3E47-1B35-1B49-A791-58A3625935F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>83</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>92</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45F657D9-0916-0C46-A470-6B510E71AB0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -26944,26 +30029,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD91425-9F4A-7E4E-B842-3368493BFFE4}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BL8" sqref="BL8"/>
+    <sheetView tabSelected="1" topLeftCell="CA3" workbookViewId="0">
+      <selection activeCell="CF8" sqref="CF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="13" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="50" customHeight="1">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -26988,8 +30074,11 @@
       <c r="I2" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" s="10" customFormat="1" ht="18" customHeight="1">
+    <row r="3" spans="1:10" s="10" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -27009,7 +30098,7 @@
         <v>16230</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -27037,8 +30126,11 @@
       <c r="I4">
         <v>19284</v>
       </c>
+      <c r="J4" s="10">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -27058,7 +30150,7 @@
         <v>15930</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -27078,7 +30170,7 @@
         <v>20133</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -27098,7 +30190,7 @@
         <v>16174</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -27118,7 +30210,7 @@
         <v>19978</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -27138,7 +30230,7 @@
         <v>21267</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -27158,7 +30250,7 @@
         <v>17520</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -27178,7 +30270,7 @@
         <v>17252</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -27206,8 +30298,11 @@
       <c r="I12">
         <v>20664</v>
       </c>
+      <c r="J12">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -27227,14 +30322,14 @@
         <v>24645</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="13" t="s">
         <v>101</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="51">
+    <row r="16" spans="1:10" ht="51">
       <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
@@ -27261,7 +30356,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -27283,7 +30378,7 @@
         <v>15645</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -27303,7 +30398,7 @@
         <v>20301</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -27323,7 +30418,7 @@
         <v>21541</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -27343,7 +30438,7 @@
         <v>22925</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -27363,7 +30458,7 @@
         <v>22739</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -27383,14 +30478,14 @@
         <v>24799</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" s="13" t="s">
         <v>92</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" ht="50" customHeight="1">
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>91</v>
       </c>
@@ -27415,8 +30510,11 @@
       <c r="I26" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="J26" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -27441,8 +30539,11 @@
       <c r="I27">
         <v>23222</v>
       </c>
+      <c r="J27">
+        <v>14</v>
+      </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -27462,7 +30563,7 @@
         <v>24698</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -27486,6 +30587,9 @@
       </c>
       <c r="I29">
         <v>20548</v>
+      </c>
+      <c r="J29">
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17">
@@ -27833,8 +30937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFFF813-639D-5044-80D4-CB11098F52B7}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -27884,7 +30988,7 @@
         <v>539</v>
       </c>
       <c r="F2" s="16">
-        <v>32.4</v>
+        <v>42.4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28">
@@ -27904,7 +31008,7 @@
         <v>245</v>
       </c>
       <c r="F3" s="18">
-        <v>39.200000000000003</v>
+        <v>49.2</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28">
@@ -28007,8 +31111,12 @@
       <c r="C11" s="18">
         <v>235</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="D11" s="18">
+        <v>4</v>
+      </c>
+      <c r="E11" s="18">
+        <v>12</v>
+      </c>
       <c r="F11" s="18">
         <v>37.200000000000003</v>
       </c>

</xml_diff>

<commit_message>
added new excel sheet to consilidate all 2017 etnp ms ms numbers
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-p2-susvsink.xlsx
+++ b/analyses/etnp2017-p2-susvsink.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905E534B-2A0E-8C42-85CB-EFCB7A8FA1CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B6DEB5-45BC-1049-BD82-83F7DF7333DD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="4240" windowWidth="27840" windowHeight="14640" activeTab="1" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="27840" windowHeight="14640" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="116">
   <si>
     <t>Sample running #</t>
   </si>
@@ -400,6 +400,9 @@
   <si>
     <t>Specific cyanobacterial peptides de novo</t>
   </si>
+  <si>
+    <t>Specific cyanobacterial peptides database</t>
+  </si>
 </sst>
 </file>
 
@@ -562,9 +565,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -575,6 +575,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1353,6 +1356,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-19C5-684D-BB7C-86F82423CFE5}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1550,6 +1556,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-19C5-684D-BB7C-86F82423CFE5}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2275,6 +2284,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-81B5-4C4F-A0DD-1058B6DA75AA}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2359,6 +2371,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-81B5-4C4F-A0DD-1058B6DA75AA}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -3558,6 +3573,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1D07-654D-A2B7-4759CA687B55}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -3576,6 +3596,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1D07-654D-A2B7-4759CA687B55}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -3639,6 +3664,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-1D07-654D-A2B7-4759CA687B55}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -3877,6 +3905,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-1D07-654D-A2B7-4759CA687B55}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9584,7 +9615,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>18</a:t>
+                      <a:t>482</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -9717,15 +9748,15 @@
           </c:yVal>
           <c:bubbleSize>
             <c:numRef>
-              <c:f>('100-965 comparison'!$J$4,'100-965 comparison'!$J$12)</c:f>
+              <c:f>('100-965 comparison'!$K$4,'100-965 comparison'!$K$12)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9790,7 +9821,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>14</a:t>
+                      <a:t>4</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -9817,7 +9848,7 @@
                   <a:p>
                     <a:r>
                       <a:rPr lang="en-US"/>
-                      <a:t>7</a:t>
+                      <a:t>0</a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
@@ -9923,15 +9954,15 @@
           </c:yVal>
           <c:bubbleSize>
             <c:numRef>
-              <c:f>('100-965 comparison'!$J$27,'100-965 comparison'!$J$29)</c:f>
+              <c:f>('100-965 comparison'!$K$27,'100-965 comparison'!$K$29)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12607,6 +12638,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5FF5-944D-A8EF-B49C51AD3DDA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -12658,6 +12694,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-5FF5-944D-A8EF-B49C51AD3DDA}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -14248,6 +14287,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-4AF6-DE41-A149-DC13035F6D06}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -28940,9 +28982,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FAA684-DE3F-5A4C-BBF8-96E0D7E03E10}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30029,10 +30071,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD91425-9F4A-7E4E-B842-3368493BFFE4}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA3" workbookViewId="0">
-      <selection activeCell="CF8" sqref="CF8"/>
+    <sheetView topLeftCell="CB2" workbookViewId="0">
+      <selection activeCell="CI3" sqref="CI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30040,16 +30082,17 @@
     <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="50" customHeight="1">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -30077,8 +30120,11 @@
       <c r="J2" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" s="10" customFormat="1" ht="18" customHeight="1">
+    <row r="3" spans="1:11" s="10" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -30098,7 +30144,7 @@
         <v>16230</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -30129,8 +30175,11 @@
       <c r="J4" s="10">
         <v>18</v>
       </c>
+      <c r="K4">
+        <v>482</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -30150,7 +30199,7 @@
         <v>15930</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -30170,7 +30219,7 @@
         <v>20133</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -30190,7 +30239,7 @@
         <v>16174</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -30210,7 +30259,7 @@
         <v>19978</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -30230,7 +30279,7 @@
         <v>21267</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -30250,7 +30299,7 @@
         <v>17520</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -30270,7 +30319,7 @@
         <v>17252</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -30301,8 +30350,11 @@
       <c r="J12">
         <v>0.01</v>
       </c>
+      <c r="K12">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -30322,14 +30374,14 @@
         <v>24645</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:11">
+      <c r="A15" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
     </row>
-    <row r="16" spans="1:10" ht="51">
+    <row r="16" spans="1:11" ht="51">
       <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
@@ -30356,7 +30408,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -30378,7 +30430,7 @@
         <v>15645</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -30398,7 +30450,7 @@
         <v>20301</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -30418,7 +30470,7 @@
         <v>21541</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -30438,7 +30490,7 @@
         <v>22925</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -30458,7 +30510,7 @@
         <v>22739</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -30478,14 +30530,14 @@
         <v>24799</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="13" t="s">
+    <row r="25" spans="1:11">
+      <c r="A25" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="50" customHeight="1">
+    <row r="26" spans="1:11" s="1" customFormat="1" ht="50" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>91</v>
       </c>
@@ -30513,8 +30565,11 @@
       <c r="J26" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="K26" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -30542,8 +30597,11 @@
       <c r="J27">
         <v>14</v>
       </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -30563,7 +30621,7 @@
         <v>24698</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -30590,6 +30648,9 @@
       </c>
       <c r="J29">
         <v>7</v>
+      </c>
+      <c r="K29">
+        <v>0.1</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17">
@@ -30938,7 +30999,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30952,98 +31013,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="12" customFormat="1" ht="88" customHeight="1" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="15">
         <v>9495</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <v>2881</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <v>18</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="15">
         <v>539</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="15">
         <v>42.4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="17">
         <v>3377</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>1294</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <v>14</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>245</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>49.2</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>2653</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>1082</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>0</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" ht="28">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>2826</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>1067</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>7</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>67</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>51.9</v>
       </c>
     </row>
@@ -31062,100 +31123,100 @@
       <c r="D7" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="88" thickBot="1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>2159</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>784</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="15">
         <v>482</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="15">
         <v>4533</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="15">
         <v>31.8</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>591</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>235</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>4</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <v>12</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>37.200000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>160</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>52</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>0</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <v>0</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6" ht="28">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="17">
         <v>1153</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>392</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>0</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>0</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
additions to p2 susvsink summary excel file
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-p2-susvsink.xlsx
+++ b/analyses/etnp2017-p2-susvsink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B6DEB5-45BC-1049-BD82-83F7DF7333DD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35892AAA-5F32-324F-A644-ACA76ADBD8D5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="27840" windowHeight="14640" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{464168A7-7287-7249-B16E-B55931B8488C}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>

</xml_diff>